<commit_message>
Converted MIP to directed Graph + added direction variable
</commit_message>
<xml_diff>
--- a/ExcelOutput/Locopos.xlsx
+++ b/ExcelOutput/Locopos.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Loco 0</t>
-  </si>
-  <si>
-    <t>Loco 1</t>
   </si>
 </sst>
 </file>
@@ -377,567 +374,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>16</v>
-      </c>
-      <c r="C6">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>16</v>
-      </c>
-      <c r="C8">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>16</v>
-      </c>
-      <c r="C15">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>16</v>
-      </c>
-      <c r="C16">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
-      <c r="C18">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
         <v>16</v>
       </c>
-      <c r="C20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
         <v>16</v>
       </c>
-      <c r="C21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
         <v>16</v>
       </c>
-      <c r="C22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
         <v>16</v>
       </c>
-      <c r="C23">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
         <v>16</v>
       </c>
-      <c r="C24">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
         <v>16</v>
       </c>
-      <c r="C25">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
         <v>16</v>
       </c>
-      <c r="C26">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>16</v>
-      </c>
-      <c r="C27">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>16</v>
-      </c>
-      <c r="C28">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>16</v>
-      </c>
-      <c r="C29">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>16</v>
-      </c>
-      <c r="C30">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>16</v>
-      </c>
-      <c r="C31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>16</v>
-      </c>
-      <c r="C32">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>16</v>
-      </c>
-      <c r="C33">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>16</v>
-      </c>
-      <c r="C34">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>16</v>
-      </c>
-      <c r="C35">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>16</v>
-      </c>
-      <c r="C36">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>16</v>
-      </c>
-      <c r="C37">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>16</v>
-      </c>
-      <c r="C38">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>16</v>
-      </c>
-      <c r="C39">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>16</v>
-      </c>
-      <c r="C40">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>16</v>
-      </c>
-      <c r="C41">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>16</v>
-      </c>
-      <c r="C42">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>16</v>
-      </c>
-      <c r="C43">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>16</v>
-      </c>
-      <c r="C44">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>16</v>
-      </c>
-      <c r="C45">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>16</v>
-      </c>
-      <c r="C46">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>16</v>
-      </c>
-      <c r="C47">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>16</v>
-      </c>
-      <c r="C48">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>16</v>
-      </c>
-      <c r="C49">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>16</v>
-      </c>
-      <c r="C50">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
-        <v>16</v>
-      </c>
-      <c r="C51">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
no sharp corners, loco
</commit_message>
<xml_diff>
--- a/ExcelOutput/Locopos.xlsx
+++ b/ExcelOutput/Locopos.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Loco 0</t>
+  </si>
+  <si>
+    <t>Loco 0 direction</t>
   </si>
 </sst>
 </file>
@@ -374,415 +377,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>145</v>
+      </c>
+      <c r="C4">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>145</v>
+      </c>
+      <c r="C5">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>142</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>158</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>159</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>160</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>161</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>174</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>35</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>173</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>172</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>133</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>94</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>96</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>130</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51">
         <v>95</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress bar GIF creation
</commit_message>
<xml_diff>
--- a/ExcelOutput/Locopos.xlsx
+++ b/ExcelOutput/Locopos.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,16 +425,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="C3">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -442,16 +442,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="C4">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="D4">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -459,16 +459,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C5">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D5">
         <v>-0</v>
       </c>
       <c r="E5">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -476,16 +476,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="D6">
         <v>-0</v>
       </c>
       <c r="E6">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -493,16 +493,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="C7">
-        <v>172</v>
+        <v>115</v>
       </c>
       <c r="D7">
         <v>-0</v>
       </c>
       <c r="E7">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -510,16 +510,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="C8">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>-0</v>
       </c>
       <c r="E8">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -527,16 +527,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="C9">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D9">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -544,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="D10">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -561,13 +561,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C11">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="D11">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>-0</v>
@@ -578,16 +578,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>172</v>
+        <v>69</v>
       </c>
       <c r="C12">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="D12">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -595,13 +595,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>173</v>
+        <v>69</v>
       </c>
       <c r="C13">
-        <v>175</v>
+        <v>114</v>
       </c>
       <c r="D13">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>-0</v>
@@ -612,13 +612,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>172</v>
+        <v>70</v>
       </c>
       <c r="C14">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E14">
         <v>-0</v>
@@ -629,10 +629,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>173</v>
+        <v>70</v>
       </c>
       <c r="C15">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>-0</v>
@@ -646,10 +646,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="C16">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D16">
         <v>-0</v>
@@ -663,10 +663,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="C17">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>-0</v>
@@ -680,10 +680,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C18">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D18">
         <v>-0</v>
@@ -697,10 +697,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C19">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D19">
         <v>-0</v>
@@ -714,10 +714,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C20">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="D20">
         <v>-0</v>
@@ -731,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C21">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="D21">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -748,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C22">
-        <v>173</v>
+        <v>69</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -765,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="C23">
-        <v>172</v>
+        <v>69</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -782,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="C24">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -799,10 +799,10 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>174</v>
+        <v>117</v>
       </c>
       <c r="C25">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D25">
         <v>-0</v>
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="C26">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -833,16 +833,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>174</v>
+        <v>119</v>
       </c>
       <c r="C27">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="D27">
         <v>-0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -850,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="C28">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="D28">
         <v>-0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -867,16 +867,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="C29">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="D29">
         <v>-0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -884,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="C30">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -901,355 +901,15 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="C31">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="1">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>174</v>
-      </c>
-      <c r="C32">
-        <v>121</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1">
-        <v>31</v>
-      </c>
-      <c r="B33">
-        <v>174</v>
-      </c>
-      <c r="C33">
-        <v>121</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1">
-        <v>32</v>
-      </c>
-      <c r="B34">
-        <v>35</v>
-      </c>
-      <c r="C34">
-        <v>121</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>173</v>
-      </c>
-      <c r="C35">
-        <v>121</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <v>172</v>
-      </c>
-      <c r="C36">
-        <v>71</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>36</v>
-      </c>
-      <c r="C37">
-        <v>132</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>132</v>
-      </c>
-      <c r="C38">
-        <v>71</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <v>71</v>
-      </c>
-      <c r="C39">
-        <v>121</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>121</v>
-      </c>
-      <c r="C40">
-        <v>120</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>121</v>
-      </c>
-      <c r="C41">
-        <v>120</v>
-      </c>
-      <c r="D41">
-        <v>-0</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>121</v>
-      </c>
-      <c r="C42">
-        <v>120</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>120</v>
-      </c>
-      <c r="C43">
-        <v>119</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>119</v>
-      </c>
-      <c r="C44">
-        <v>118</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>120</v>
-      </c>
-      <c r="C45">
-        <v>118</v>
-      </c>
-      <c r="D45">
-        <v>-0</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>120</v>
-      </c>
-      <c r="C46">
-        <v>117</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1">
-        <v>45</v>
-      </c>
-      <c r="B47">
-        <v>120</v>
-      </c>
-      <c r="C47">
-        <v>117</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1">
-        <v>46</v>
-      </c>
-      <c r="B48">
-        <v>120</v>
-      </c>
-      <c r="C48">
-        <v>116</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1">
-        <v>47</v>
-      </c>
-      <c r="B49">
-        <v>119</v>
-      </c>
-      <c r="C49">
-        <v>116</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1">
-        <v>48</v>
-      </c>
-      <c r="B50">
-        <v>120</v>
-      </c>
-      <c r="C50">
-        <v>116</v>
-      </c>
-      <c r="D50">
-        <v>-0</v>
-      </c>
-      <c r="E50">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51">
-        <v>120</v>
-      </c>
-      <c r="C51">
-        <v>115</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51">
         <v>1</v>
       </c>
     </row>

</xml_diff>